<commit_message>
Began Tr2 and updated Corpus Header
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Hand1</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>General suspension dot</t>
+  </si>
+  <si>
+    <t>g10</t>
+  </si>
+  <si>
+    <t>acht/sed abbreviation</t>
   </si>
 </sst>
 </file>
@@ -768,10 +774,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,6 +852,14 @@
       </c>
       <c r="B9" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T9 ongoing (plus other changes)
Commas are now used to seperate multiple attribute values throughout the corpus.
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>Hand1</t>
   </si>
@@ -226,9 +226,6 @@
     <t>g6</t>
   </si>
   <si>
-    <t>ir superscript</t>
-  </si>
-  <si>
     <t>num</t>
   </si>
   <si>
@@ -338,6 +335,33 @@
   </si>
   <si>
     <t>uir abbreviation</t>
+  </si>
+  <si>
+    <t>Hand9</t>
+  </si>
+  <si>
+    <t>Eoghan Mac Gilleoin</t>
+  </si>
+  <si>
+    <t>Hand10</t>
+  </si>
+  <si>
+    <t>Niall Mac Mhuirich</t>
+  </si>
+  <si>
+    <t>Transcription 9</t>
+  </si>
+  <si>
+    <t>Transcription 12</t>
+  </si>
+  <si>
+    <t>g20</t>
+  </si>
+  <si>
+    <t>Superscript e</t>
+  </si>
+  <si>
+    <t>Superscript ir</t>
   </si>
 </sst>
 </file>
@@ -741,10 +765,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC96CB5E-8856-4282-8506-D0186FBEACCB}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,10 +858,32 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" t="s">
         <v>64</v>
       </c>
-      <c r="C8" t="s">
-        <v>65</v>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -891,7 +937,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -911,20 +957,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
-      </c>
-      <c r="B1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -948,7 +994,7 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -972,111 +1018,119 @@
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="s">
         <v>56</v>
-      </c>
-      <c r="B8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
         <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" t="s">
         <v>60</v>
-      </c>
-      <c r="B10" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
         <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" t="s">
         <v>70</v>
-      </c>
-      <c r="B12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
         <v>74</v>
-      </c>
-      <c r="B13" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" t="s">
         <v>78</v>
-      </c>
-      <c r="B15" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
         <v>80</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" t="s">
         <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
         <v>87</v>
-      </c>
-      <c r="B19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
-        <v>91</v>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1151,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
@@ -1157,22 +1211,22 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transcription and Stylesheet Work
I haven't committed in a while, so there are lots of changes.
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="4" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
   <sheets>
     <sheet name="Resps" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="ana" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="123">
   <si>
     <t>Hand1</t>
   </si>
@@ -419,6 +420,18 @@
   </si>
   <si>
     <t>ptcp</t>
+  </si>
+  <si>
+    <t>g29</t>
+  </si>
+  <si>
+    <t>Superscript t</t>
+  </si>
+  <si>
+    <t>g30</t>
+  </si>
+  <si>
+    <t>q abbreviation</t>
   </si>
 </sst>
 </file>
@@ -1014,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1252,6 +1265,22 @@
       </c>
       <c r="B29" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1264,7 +1293,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454430F-1798-4EA5-9464-01065034EA9C}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
T9, JS, and Corpus Work
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="4" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
   <sheets>
     <sheet name="Resps" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
   <si>
     <t>Hand1</t>
   </si>
@@ -464,6 +464,15 @@
   </si>
   <si>
     <t>Superscript l</t>
+  </si>
+  <si>
+    <t>g32</t>
+  </si>
+  <si>
+    <t>et reliqua</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1362,6 +1371,14 @@
       </c>
       <c r="B32" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>134</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1372,10 +1389,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454430F-1798-4EA5-9464-01065034EA9C}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,6 +1490,11 @@
         <v>117</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>136</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
T9 and JS Work
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="4" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
   <sheets>
     <sheet name="Resps" sheetId="3" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
   <si>
     <t>Hand1</t>
   </si>
@@ -473,6 +473,12 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>g33</t>
+  </si>
+  <si>
+    <t>Vertical m</t>
   </si>
 </sst>
 </file>
@@ -1109,10 +1115,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,6 +1385,14 @@
       </c>
       <c r="B33" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1391,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454430F-1798-4EA5-9464-01065034EA9C}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
T7, T9 and ongoing JS work
NB. stylesheets unfinished
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
   <si>
     <t>Hand1</t>
   </si>
@@ -479,6 +479,12 @@
   </si>
   <si>
     <t>Vertical m</t>
+  </si>
+  <si>
+    <t>g34</t>
+  </si>
+  <si>
+    <t>pro abbreviation</t>
   </si>
 </sst>
 </file>
@@ -1115,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1393,6 +1399,14 @@
       </c>
       <c r="B34" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transcription, JS work, and stylesheet rewrite
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
   <si>
     <t>Hand1</t>
   </si>
@@ -485,6 +485,30 @@
   </si>
   <si>
     <t>pro abbreviation</t>
+  </si>
+  <si>
+    <t>g35</t>
+  </si>
+  <si>
+    <t>ligature</t>
+  </si>
+  <si>
+    <t>g36</t>
+  </si>
+  <si>
+    <t>ac ligature</t>
+  </si>
+  <si>
+    <t>p with tail</t>
+  </si>
+  <si>
+    <t>g37</t>
+  </si>
+  <si>
+    <t>g38</t>
+  </si>
+  <si>
+    <t>ur abbreviation</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1145,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,6 +1431,38 @@
       </c>
       <c r="B35" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>141</v>
+      </c>
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T5 work and minor stylesheet work
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="161">
   <si>
     <t>Hand1</t>
   </si>
@@ -521,6 +521,30 @@
   </si>
   <si>
     <t>Superscript b</t>
+  </si>
+  <si>
+    <t>g41</t>
+  </si>
+  <si>
+    <t>l with suspension stroke</t>
+  </si>
+  <si>
+    <t>Hand 15</t>
+  </si>
+  <si>
+    <t>Unk. Hand in NLS Adv. MS. 72.1.33</t>
+  </si>
+  <si>
+    <t>g42</t>
+  </si>
+  <si>
+    <t>Superscript s</t>
+  </si>
+  <si>
+    <t>g43</t>
+  </si>
+  <si>
+    <t>Subscript i</t>
   </si>
 </sst>
 </file>
@@ -924,10 +948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC96CB5E-8856-4282-8506-D0186FBEACCB}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,6 +1107,17 @@
         <v>131</v>
       </c>
       <c r="C14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1157,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1491,6 +1526,30 @@
       </c>
       <c r="B41" t="s">
         <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stylesheet and T5 work
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="174">
   <si>
     <t>Hand1</t>
   </si>
@@ -376,9 +376,6 @@
     <t>tit</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>g23</t>
   </si>
   <si>
@@ -563,6 +560,30 @@
   </si>
   <si>
     <t>ir abbreviation</t>
+  </si>
+  <si>
+    <t>Hand16</t>
+  </si>
+  <si>
+    <t>Hand17</t>
+  </si>
+  <si>
+    <t>Hand18</t>
+  </si>
+  <si>
+    <t>Rev. John Beaton</t>
+  </si>
+  <si>
+    <t>Neil Beaton</t>
+  </si>
+  <si>
+    <t>Dubhghall Albanach mac mhic Cathail</t>
+  </si>
+  <si>
+    <t>Transcription 4</t>
+  </si>
+  <si>
+    <t>prep</t>
   </si>
 </sst>
 </file>
@@ -966,10 +987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC96CB5E-8856-4282-8506-D0186FBEACCB}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1094,7 @@
         <v>92</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1081,62 +1102,98 @@
         <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B11" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="C11" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B12" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" t="s">
         <v>125</v>
-      </c>
-      <c r="C12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" t="s">
         <v>130</v>
       </c>
-      <c r="B14" t="s">
-        <v>131</v>
-      </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B15" t="s">
         <v>155</v>
       </c>
-      <c r="B15" t="s">
-        <v>156</v>
-      </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>166</v>
+      </c>
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" t="s">
+        <v>171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1212,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
   <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,194 +1461,194 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" t="s">
         <v>105</v>
-      </c>
-      <c r="B24" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B26" t="s">
         <v>109</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B27" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>112</v>
+      </c>
+      <c r="B28" t="s">
         <v>113</v>
-      </c>
-      <c r="B28" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" t="s">
         <v>115</v>
-      </c>
-      <c r="B29" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B30" t="s">
         <v>118</v>
-      </c>
-      <c r="B30" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" t="s">
         <v>120</v>
-      </c>
-      <c r="B31" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" t="s">
         <v>132</v>
-      </c>
-      <c r="B32" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B33" t="s">
         <v>134</v>
-      </c>
-      <c r="B33" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" t="s">
         <v>137</v>
-      </c>
-      <c r="B34" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" t="s">
         <v>139</v>
-      </c>
-      <c r="B35" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" t="s">
         <v>141</v>
-      </c>
-      <c r="B36" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" t="s">
         <v>147</v>
-      </c>
-      <c r="B39" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B40" t="s">
         <v>149</v>
-      </c>
-      <c r="B40" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" t="s">
         <v>151</v>
-      </c>
-      <c r="B41" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>152</v>
+      </c>
+      <c r="B42" t="s">
         <v>153</v>
-      </c>
-      <c r="B42" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" t="s">
         <v>157</v>
-      </c>
-      <c r="B43" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>158</v>
+      </c>
+      <c r="B44" t="s">
         <v>159</v>
-      </c>
-      <c r="B44" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>160</v>
+      </c>
+      <c r="B45" t="s">
         <v>161</v>
-      </c>
-      <c r="B45" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" t="s">
         <v>163</v>
-      </c>
-      <c r="B46" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>164</v>
+      </c>
+      <c r="B47" t="s">
         <v>165</v>
-      </c>
-      <c r="B47" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1602,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C454430F-1798-4EA5-9464-01065034EA9C}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1690,22 +1747,24 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>103</v>
       </c>
-      <c r="B17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T2, T13, and Stylesheet work
Handling of <choice> situations fine-tuned.
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="180">
   <si>
     <t>Hand1</t>
   </si>
@@ -596,6 +596,12 @@
   </si>
   <si>
     <t>uir (curly descender with cross-stroke)</t>
+  </si>
+  <si>
+    <t>g49</t>
+  </si>
+  <si>
+    <t>k abbreviation</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B49"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1677,6 +1683,14 @@
       </c>
       <c r="B49" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>178</v>
+      </c>
+      <c r="B50" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T4 and Stylesheet Work
Improved handling of <lb> elements so that the line number is displayed in all contexts.
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,8 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\faclair-manuscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{60D88FB1-25E8-40EC-8825-1E042793E2CC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
   <sheets>
     <sheet name="Resps" sheetId="3" r:id="rId1"/>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="182">
   <si>
     <t>Hand1</t>
   </si>
@@ -602,6 +603,12 @@
   </si>
   <si>
     <t>k abbreviation</t>
+  </si>
+  <si>
+    <t>g50</t>
+  </si>
+  <si>
+    <t>apostrophe</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1292,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1691,6 +1698,14 @@
       </c>
       <c r="B50" t="s">
         <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>180</v>
+      </c>
+      <c r="B51" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
T14, T4, and Stylesheet Work
Made handling of <add> elements less overly specific.
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\faclair-manuscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{6FD2D490-1D34-4A59-ACEE-1D3DCD3A9575}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D51E4D03-4653-4D2E-8330-211C00D4119B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="1" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
   <sheets>
     <sheet name="Resps" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Glyphs" sheetId="4" r:id="rId4"/>
     <sheet name="ana" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
   <si>
     <t>Hand1</t>
   </si>
@@ -609,6 +609,15 @@
   </si>
   <si>
     <t>apostrophe</t>
+  </si>
+  <si>
+    <t>Hand19</t>
+  </si>
+  <si>
+    <t>Eoin mac Domhnaill Ó Conchubuir</t>
+  </si>
+  <si>
+    <t>Transcription 14</t>
   </si>
 </sst>
 </file>
@@ -1012,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC96CB5E-8856-4282-8506-D0186FBEACCB}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1219,6 +1228,17 @@
       </c>
       <c r="C18" t="s">
         <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -1294,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
T13 complete; T4 corrections
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\faclair-manuscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6CCD3C36-963F-43AF-8418-D49B67B70CDF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BD0E6FD-4B60-4BB3-B87C-7135F5F88E51}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
@@ -629,7 +629,7 @@
     <t>g52</t>
   </si>
   <si>
-    <t>diagonal overstrokr</t>
+    <t>diagonal overstroke</t>
   </si>
 </sst>
 </file>
@@ -1326,7 +1326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrections, T3, and Stylesheet Work
- Mass correction of an incorrect URL for "agus" (!).
- XML-to-XML process set up for extracting a database of headwords from the transcription files, then updating it with new headwords. It is envisaged that this will be drawn upon for extra data on headwords (e.g. gender, stem etc.).
</commit_message>
<xml_diff>
--- a/xmlid lists.xlsx
+++ b/xmlid lists.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\faclair-manuscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DC95496-E9BA-45E7-B5C7-B6C55A87718B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7BCE5CA6-40EC-432E-934D-2F745C989255}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" activeTab="3" xr2:uid="{F2FD37ED-5505-4273-997E-CED0D63E6282}"/>
   </bookViews>
@@ -1353,7 +1353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CC8ACE-6DAF-46E3-8EE2-C041D28A1119}">
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>

</xml_diff>